<commit_message>
adding some magic :)
</commit_message>
<xml_diff>
--- a/db/database.xlsx
+++ b/db/database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>user</t>
   </si>
@@ -97,6 +97,45 @@
   </si>
   <si>
     <t>DATABASE VER 0.1</t>
+  </si>
+  <si>
+    <t>TABELS</t>
+  </si>
+  <si>
+    <t>NAMA TABEL</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>INT25</t>
+  </si>
+  <si>
+    <t>VARCHAR60</t>
+  </si>
+  <si>
+    <t>VARCHAR30</t>
+  </si>
+  <si>
+    <t>INT11</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>VARCHAR100</t>
+  </si>
+  <si>
+    <t>INT15</t>
+  </si>
+  <si>
+    <t>LONGTEXT</t>
+  </si>
+  <si>
+    <t>UTF8_general_ci</t>
   </si>
 </sst>
 </file>
@@ -270,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -287,6 +326,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,67 +626,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E27"/>
+  <dimension ref="B1:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:5" ht="15.75" thickBot="1">
+    <row r="1" spans="2:9">
+      <c r="B1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:9" ht="15.75" thickBot="1">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="23.25">
+    <row r="4" spans="2:9" ht="23.25">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="2:5">
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:5">
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="2:5">
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="2:5">
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="2:5">
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -652,8 +745,11 @@
         <v>8</v>
       </c>
       <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="2:5" ht="15.75" thickBot="1">
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="15.75" thickBot="1">
       <c r="D11" s="8">
         <v>1</v>
       </c>
@@ -661,7 +757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:9">
       <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
@@ -672,7 +768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:9">
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
@@ -682,8 +778,11 @@
       <c r="E13" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="2:5">
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
@@ -693,8 +792,14 @@
       <c r="E14" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="2:5">
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
@@ -704,29 +809,47 @@
       <c r="E15" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="2:5">
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:5">
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
       <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" thickBot="1"/>
-    <row r="20" spans="2:5">
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="15.75" thickBot="1"/>
+    <row r="20" spans="2:9">
       <c r="B20" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:9">
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:5">
+      <c r="G21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
@@ -737,8 +860,11 @@
         <v>21</v>
       </c>
       <c r="E22" s="14"/>
-    </row>
-    <row r="23" spans="2:5">
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
       <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
@@ -748,8 +874,14 @@
       <c r="E23" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="2:5">
+      <c r="G23" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
       <c r="D24" s="8">
         <v>2</v>
       </c>
@@ -757,7 +889,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:9">
       <c r="D25" s="10">
         <v>3</v>
       </c>
@@ -765,15 +897,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:9">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:9">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added missing magic :D , default thing
</commit_message>
<xml_diff>
--- a/db/database.xlsx
+++ b/db/database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>user</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>UTF8_general_ci</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
   </si>
 </sst>
 </file>
@@ -628,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -653,6 +656,9 @@
       <c r="G1" t="s">
         <v>29</v>
       </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
       <c r="I1" t="s">
         <v>30</v>
       </c>
@@ -733,6 +739,9 @@
       <c r="G9" t="s">
         <v>34</v>
       </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="4" t="s">
@@ -862,6 +871,9 @@
       <c r="E22" s="14"/>
       <c r="G22" t="s">
         <v>34</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:9">

</xml_diff>

<commit_message>
fixing the database architecture :(
</commit_message>
<xml_diff>
--- a/db/database.xlsx
+++ b/db/database.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>user</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>OwnerFn</t>
   </si>
   <si>
@@ -36,9 +33,6 @@
     <t>Partnership</t>
   </si>
   <si>
-    <t>*UserID</t>
-  </si>
-  <si>
     <t>company</t>
   </si>
   <si>
@@ -72,15 +66,9 @@
     <t>Introduction</t>
   </si>
   <si>
-    <t>^UserID</t>
-  </si>
-  <si>
     <t>Content</t>
   </si>
   <si>
-    <t>PostID</t>
-  </si>
-  <si>
     <t>PostCat</t>
   </si>
   <si>
@@ -93,9 +81,6 @@
     <t>Blog</t>
   </si>
   <si>
-    <t>------------</t>
-  </si>
-  <si>
     <t>DATABASE VER 0.1</t>
   </si>
   <si>
@@ -139,6 +124,30 @@
   </si>
   <si>
     <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>²Username</t>
+  </si>
+  <si>
+    <t>*UID</t>
+  </si>
+  <si>
+    <t>*CID</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Primerykey</t>
+  </si>
+  <si>
+    <t>²</t>
+  </si>
+  <si>
+    <t>Foreginkey</t>
+  </si>
+  <si>
+    <t>*PID</t>
   </si>
 </sst>
 </file>
@@ -342,6 +351,377 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>106363</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1571625" y="1943100"/>
+          <a:ext cx="466725" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="lgDash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>106363</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1562100" y="4438650"/>
+          <a:ext cx="466725" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="lgDash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247651</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>523876</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Connector 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="247651" y="962025"/>
+          <a:ext cx="276225" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Connector 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="-614362" y="1814512"/>
+          <a:ext cx="1743075" cy="38100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>96838</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="2705100"/>
+          <a:ext cx="257175" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1581150" y="971550"/>
+          <a:ext cx="276225" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Connector 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="214313" y="2586037"/>
+          <a:ext cx="3248025" cy="57150"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="1552576" y="4229099"/>
+          <a:ext cx="257175" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -631,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -646,21 +1026,21 @@
   <sheetData>
     <row r="1" spans="2:9">
       <c r="B1" s="16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="15.75" thickBot="1"/>
@@ -671,91 +1051,102 @@
     </row>
     <row r="4" spans="2:9" ht="23.25">
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
         <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
+      <c r="I9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>25</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C10" s="12"/>
       <c r="D10" s="13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1">
@@ -763,155 +1154,171 @@
         <v>1</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12" s="8">
         <v>2</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D13" s="8">
         <v>3</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D14" s="8">
         <v>4</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="10">
         <v>5</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I16" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="3" t="s">
-        <v>16</v>
+      <c r="B17" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="I17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="20" spans="2:9">
       <c r="B20" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="G21" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:9">
       <c r="B22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="14"/>
+        <v>36</v>
+      </c>
+      <c r="C22" s="12"/>
       <c r="G22" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
+      <c r="I22" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="23" spans="2:9">
-      <c r="B23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="8">
+      <c r="B23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="G23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="8">
         <v>1</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9">
-      <c r="D24" s="8">
+      <c r="E24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="D25" s="8">
         <v>2</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9">
-      <c r="D25" s="10">
+      <c r="E25" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="D26" s="10">
         <v>3</v>
       </c>
-      <c r="E25" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9">
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="E26" s="11" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="2:9">
       <c r="D27" s="5"/>
@@ -923,6 +1330,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>